<commit_message>
Updated OVWDemo Sheets for productListing and serviceListing.
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_service_listing.xlsx
+++ b/docs/OVW Sheets/OVWDemo_service_listing.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755" activeTab="47"/>
   </bookViews>
   <sheets>
     <sheet name="de_de" sheetId="1" r:id="rId1"/>
@@ -62,7 +57,7 @@
     <sheet name="fr_be" sheetId="48" r:id="rId48"/>
     <sheet name="Sheet25" sheetId="49" r:id="rId49"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -72,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="235">
   <si>
     <t>http://www.cisco.com/web/DE/solutions/collaboration/services.html</t>
   </si>
@@ -249,9 +244,6 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/BE/nl/products/security/services.html</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>http://www.cisco.com/web/BG/solutions/borderless/services.html</t>
@@ -870,7 +862,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -883,7 +875,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -945,7 +936,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -980,7 +971,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1157,7 +1148,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1199,7 +1190,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1303,7 +1294,7 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1370,9 +1361,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1383,7 +1376,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1396,68 +1389,39 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>59</v>
+      <c r="A2" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/products/servers-unified-computing/service-listing.html"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="A1" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="A1" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1480,7 +1444,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1494,10 +1458,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1508,7 +1472,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -1522,7 +1486,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -1536,7 +1500,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -1577,7 +1541,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1591,10 +1555,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1605,7 +1569,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -1619,7 +1583,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -1633,7 +1597,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -1676,7 +1640,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1690,10 +1654,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1704,7 +1668,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -1718,7 +1682,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -1732,7 +1696,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -1773,7 +1737,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
@@ -1788,10 +1752,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>13</v>
@@ -1803,7 +1767,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>16</v>
@@ -1818,7 +1782,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>18</v>
@@ -1833,7 +1797,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>20</v>
@@ -1862,10 +1826,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1842,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1892,26 +1856,26 @@
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>59</v>
+      <c r="A2" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1920,45 +1884,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/products/servers-unified-computing/service-listing.html"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
-    <hyperlink ref="A5" r:id="rId3" display="http://www.cisco.com/web/DE/products/security/services.html"/>
-    <hyperlink ref="A4" r:id="rId4"/>
-    <hyperlink ref="A3" r:id="rId5"/>
-    <hyperlink ref="A1" r:id="rId6"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="A1" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1982,7 +1914,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1997,10 +1929,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2012,7 +1944,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -2027,7 +1959,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -2042,7 +1974,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -2085,7 +2017,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2100,10 +2032,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2115,7 +2047,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -2130,7 +2062,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -2145,7 +2077,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -2188,7 +2120,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2203,10 +2135,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2218,7 +2150,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -2233,7 +2165,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -2248,7 +2180,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -2309,7 +2241,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2390,7 +2322,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2405,10 +2337,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2420,7 +2352,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -2435,7 +2367,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -2450,7 +2382,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -2479,10 +2411,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E1:E6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,7 +2425,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2507,26 +2439,26 @@
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>59</v>
+      <c r="A2" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -2535,44 +2467,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/products/servers-unified-computing/service-listing.html"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="A1" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="A1" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2580,10 +2481,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E1:E5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2594,7 +2495,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2609,10 +2510,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2624,7 +2525,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -2639,7 +2540,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -2651,21 +2552,6 @@
         <v>3</v>
       </c>
       <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2696,7 +2582,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2711,10 +2597,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2726,7 +2612,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -2741,7 +2627,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -2756,7 +2642,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -2801,7 +2687,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2816,10 +2702,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2831,7 +2717,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -2846,7 +2732,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -2861,7 +2747,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -2890,10 +2776,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2907,7 +2793,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2921,17 +2807,17 @@
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>59</v>
+      <c r="A2" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E2" s="6"/>
     </row>
@@ -2940,7 +2826,7 @@
         <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -2949,44 +2835,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/products/servers-unified-computing/service-listing.html"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
-    <hyperlink ref="A1" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
+    <hyperlink ref="A1" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
     <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2994,10 +2849,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3011,7 +2866,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3023,32 +2878,32 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>59</v>
-      </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>235</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>128</v>
+      <c r="A3" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -3057,55 +2912,18 @@
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/products/servers-unified-computing/service-listing.html"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
-    <hyperlink ref="E1" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4" display="http://www.cisco.com/c/en/us/products/servers-unified-computing/service-listing.html"/>
-    <hyperlink ref="E5" r:id="rId5"/>
-    <hyperlink ref="E4" r:id="rId6"/>
-    <hyperlink ref="E3" r:id="rId7"/>
-    <hyperlink ref="A1" r:id="rId8"/>
-    <hyperlink ref="A3" r:id="rId9"/>
-    <hyperlink ref="A4" r:id="rId10"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
+    <hyperlink ref="E1" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="A1" r:id="rId5"/>
+    <hyperlink ref="A2" r:id="rId6"/>
+    <hyperlink ref="A3" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3130,7 +2948,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3142,15 +2960,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -3159,12 +2977,12 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -3176,12 +2994,12 @@
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -3193,12 +3011,12 @@
         <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -3210,7 +3028,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3251,7 +3069,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3263,15 +3081,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -3280,12 +3098,12 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -3297,12 +3115,12 @@
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -3314,12 +3132,12 @@
         <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -3331,7 +3149,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3357,7 +3175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
@@ -3372,7 +3190,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3387,10 +3205,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -3402,7 +3220,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -3417,7 +3235,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -3432,7 +3250,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -3490,7 +3308,7 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -3551,7 +3369,7 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
@@ -3623,7 +3441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
@@ -3638,7 +3456,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3653,10 +3471,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -3668,7 +3486,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -3683,7 +3501,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -3698,7 +3516,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -3744,7 +3562,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3756,15 +3574,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -3773,12 +3591,12 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -3790,12 +3608,12 @@
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -3807,12 +3625,12 @@
         <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -3824,7 +3642,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3850,7 +3668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E7"/>
     </sheetView>
   </sheetViews>
@@ -3865,7 +3683,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3880,10 +3698,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -3895,7 +3713,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -3910,7 +3728,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -3925,7 +3743,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -3971,7 +3789,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3983,15 +3801,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -4000,12 +3818,12 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -4017,12 +3835,12 @@
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -4034,12 +3852,12 @@
         <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -4051,7 +3869,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -4092,7 +3910,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -4104,15 +3922,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -4121,12 +3939,12 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -4138,12 +3956,12 @@
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -4155,12 +3973,12 @@
         <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -4172,7 +3990,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -4213,7 +4031,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -4225,15 +4043,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -4242,12 +4060,12 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -4259,12 +4077,12 @@
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -4276,12 +4094,12 @@
         <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -4293,7 +4111,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -4317,10 +4135,10 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4334,7 +4152,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -4346,22 +4164,24 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>235</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4369,7 +4189,7 @@
         <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -4378,53 +4198,18 @@
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/products/servers-unified-computing/service-listing.html"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
-    <hyperlink ref="E1" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4" display="http://www.cisco.com/c/en/us/products/servers-unified-computing/service-listing.html"/>
-    <hyperlink ref="E3" r:id="rId5"/>
-    <hyperlink ref="E5" r:id="rId6"/>
-    <hyperlink ref="E4" r:id="rId7"/>
-    <hyperlink ref="A1" r:id="rId8"/>
-    <hyperlink ref="A3" r:id="rId9"/>
-    <hyperlink ref="A4" r:id="rId10"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
+    <hyperlink ref="E1" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="A1" r:id="rId5"/>
+    <hyperlink ref="A2" r:id="rId6"/>
+    <hyperlink ref="A3" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4449,7 +4234,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -4461,15 +4246,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -4478,12 +4263,12 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -4495,12 +4280,12 @@
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -4512,12 +4297,12 @@
         <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -4529,7 +4314,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -4555,7 +4340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
@@ -4570,7 +4355,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -4585,10 +4370,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -4600,7 +4385,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -4615,7 +4400,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -4630,7 +4415,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -4674,7 +4459,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -4689,10 +4474,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -4704,7 +4489,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -4719,7 +4504,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -4734,7 +4519,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -4795,7 +4580,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -4879,7 +4664,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -4894,10 +4679,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -4909,7 +4694,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -4924,7 +4709,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -4939,7 +4724,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -4970,7 +4755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
@@ -4985,7 +4770,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5000,10 +4785,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -5015,7 +4800,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -5030,7 +4815,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -5045,7 +4830,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -5076,7 +4861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
@@ -5091,7 +4876,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5106,10 +4891,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -5121,7 +4906,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -5136,7 +4921,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -5151,7 +4936,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -5182,7 +4967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
@@ -5197,7 +4982,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5212,10 +4997,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -5227,7 +5012,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -5242,7 +5027,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -5257,7 +5042,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -5286,10 +5071,10 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5303,7 +5088,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5318,10 +5103,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -5332,11 +5117,11 @@
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>59</v>
+      <c r="A3" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -5345,44 +5130,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://www.cisco.com/c/en/us/products/servers-unified-computing/service-listing.html"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://www.cisco.com/c/en/us/solutions/data-center-virtualization/service-listing.html"/>
-    <hyperlink ref="A1" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="A1" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="A3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5392,7 +5146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
@@ -5407,7 +5161,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5422,10 +5176,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -5437,7 +5191,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -5452,7 +5206,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -5467,7 +5221,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -5498,7 +5252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -5513,7 +5267,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5528,10 +5282,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -5543,7 +5297,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -5558,7 +5312,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -5573,7 +5327,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -5616,7 +5370,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5631,10 +5385,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -5646,7 +5400,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -5661,7 +5415,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -5676,7 +5430,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -5707,7 +5461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
@@ -5720,7 +5474,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5735,10 +5489,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -5750,7 +5504,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -5765,7 +5519,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -5780,7 +5534,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -5853,7 +5607,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -5952,7 +5706,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -6051,7 +5805,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -6150,7 +5904,7 @@
         <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -6219,7 +5973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6249,7 +6003,7 @@
         <v>53</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>

</xml_diff>